<commit_message>
Add shortcuts and update translations
</commit_message>
<xml_diff>
--- a/src/locales/i18n.xlsx
+++ b/src/locales/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>key</t>
   </si>
@@ -34,10 +34,16 @@
     <t>编辑文章</t>
   </si>
   <si>
-    <t>Skip</t>
-  </si>
-  <si>
-    <t>跳过</t>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>下一个</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>上一个</t>
   </si>
   <si>
     <t>ToggleSimple</t>
@@ -58,6 +64,12 @@
     <t>下一章</t>
   </si>
   <si>
+    <t>PreviousChapter</t>
+  </si>
+  <si>
+    <t>上一章</t>
+  </si>
+  <si>
     <t>RepeatChapter</t>
   </si>
   <si>
@@ -70,7 +82,7 @@
     <t>默写本章</t>
   </si>
   <si>
-    <t>PlaySound</t>
+    <t>PlayWordPronunciation</t>
   </si>
   <si>
     <t>播放发音</t>
@@ -514,10 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z200"/>
+  <dimension ref="A1:Z202"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="26" width="19.950000000000003" customWidth="1"/>
+    <col min="1" max="1" width="22.61" customWidth="1"/>
+    <col min="2" max="26" width="19.950000000000003" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -651,8 +664,22 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="19" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
     <row r="20" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
     <row r="21" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
@@ -835,6 +862,8 @@
     <row r="198" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
     <row r="199" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
     <row r="200" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Improve the dictionary of nce2 articles
</commit_message>
<xml_diff>
--- a/src/locales/i18n.xlsx
+++ b/src/locales/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>key</t>
   </si>
@@ -122,6 +122,30 @@
   </si>
   <si>
     <t>切换简洁模式</t>
+  </si>
+  <si>
+    <t>TogglePanel</t>
+  </si>
+  <si>
+    <t>显示/隐藏列表</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>中文</t>
+  </si>
+  <si>
+    <t>英语</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>德语</t>
+  </si>
+  <si>
+    <t>zh-CN</t>
   </si>
 </sst>
 </file>
@@ -680,11 +704,46 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="24" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
     <row r="25" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>
     <row r="26" ht="18.045112781954888" customHeight="1" spans="1:26" x14ac:dyDescent="0.25"/>

</xml_diff>